<commit_message>
pom project update sequences
</commit_message>
<xml_diff>
--- a/data/moje-data.xlsx
+++ b/data/moje-data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500"/>
+    <workbookView xWindow="1540" yWindow="6560" windowWidth="14400" windowHeight="9660" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="16">
   <si>
     <t>P1</t>
   </si>
@@ -72,16 +72,25 @@
   </si>
   <si>
     <t>SQ</t>
+  </si>
+  <si>
+    <t>[Sequence: [P1,P3,P4,], Sequence: [P2,P3,P5,P6,], Sequence: [P2,P3,P4,P5,]]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -92,19 +101,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -115,6 +123,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -131,15 +157,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -476,362 +509,408 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="210" zoomScaleNormal="210" zoomScalePageLayoutView="210" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="128" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
+      <c r="B1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+    </row>
+    <row r="3" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="1"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="4"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
       <c r="I5" t="s">
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
+      <c r="A6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2"/>
       <c r="I6" t="s">
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
+      <c r="A7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="2"/>
       <c r="I7" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
+      <c r="A8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
       <c r="I8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J8" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="I10" t="s">
         <v>2</v>
       </c>
       <c r="J10" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>14</v>
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="I11" t="s">
         <v>2</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
       <c r="I12" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J12" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="I13" t="s">
+        <v>2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>2</v>
+      </c>
+      <c r="J14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" t="s">
         <v>3</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I14" s="3" t="s">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I15" s="3" t="s">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J15" t="s">
+      <c r="J18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="I16" s="3" t="s">
+    <row r="19" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J16" t="s">
+      <c r="J19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I17" s="3" t="s">
+    <row r="20" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J17" t="s">
+      <c r="J20" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I18" s="3" t="s">
+    <row r="21" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J21" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I19" s="3" t="s">
+    <row r="22" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J19" t="s">
+      <c r="J22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I20" s="3" t="s">
+    <row r="23" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I23" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J20" t="s">
+      <c r="J23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I21" s="3" t="s">
+    <row r="24" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I24" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J21" t="s">
+      <c r="J24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I22" s="3" t="s">
+    <row r="25" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I25" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J22" t="s">
+      <c r="J25" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I23" s="3" t="s">
+    <row r="26" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I26" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I24" s="3" t="s">
+    <row r="27" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I27" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J24" t="s">
+      <c r="J27" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I25" s="3" t="s">
+    <row r="28" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I28" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J28" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I26" s="3" t="s">
+    <row r="29" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="30" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I30" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J26" t="s">
+      <c r="J30" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I27" s="3" t="s">
+    <row r="31" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I31" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J27" t="s">
+      <c r="J31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="9:10" x14ac:dyDescent="0.2">
-      <c r="I28" s="3" t="s">
+    <row r="32" spans="9:10" x14ac:dyDescent="0.2">
+      <c r="I32" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J32" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>